<commit_message>
set Export Demand to 10 (2030) and 50 (2050) PJ
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCC02A6-372D-47A4-B1D0-449539B1C33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E571A457-5F66-4EA7-A0B0-4D643B1E1287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
@@ -211,7 +212,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,8 +220,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -249,8 +251,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
+    <cellStyle name="Comma" xfId="7" builtinId="3"/>
     <cellStyle name="Komma 12" xfId="2" xr:uid="{8F711D16-269A-4836-8933-8B8AF3944FE9}"/>
     <cellStyle name="Neutral 3" xfId="3" xr:uid="{5B3B309E-6B7E-4D77-AD41-EB17FF9CE808}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,19 +543,19 @@
   <dimension ref="C2:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y11:Y12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -561,7 +566,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
@@ -577,7 +582,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
@@ -615,7 +620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D5">
         <v>2030</v>
       </c>
@@ -625,17 +630,21 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
+        <v>10</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>2045</v>
       </c>
@@ -645,17 +654,21 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <v>50</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15">
         <v>0</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -667,7 +680,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -679,7 +692,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -693,7 +706,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -707,7 +720,7 @@
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -721,7 +734,7 @@
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -735,7 +748,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -749,7 +762,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -763,7 +776,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="17" spans="20:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="20:31" x14ac:dyDescent="0.3">
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>

</xml_diff>

<commit_message>
Include 2050 into Export Demand
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E571A457-5F66-4EA7-A0B0-4D643B1E1287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66921E78-92E5-44A4-9D66-FA0B9423BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -543,7 +543,7 @@
   <dimension ref="C2:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,15 +670,28 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="D7">
+        <v>2050</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
+        <v>50</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>

</xml_diff>

<commit_message>
Update Export Demand in SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx and co2 transport in SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsH2ExportDemand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66921E78-92E5-44A4-9D66-FA0B9423BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5738CF79-86DA-4521-86BD-46E01278C10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8628" yWindow="3696" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -94,7 +94,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,12 +133,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -216,13 +210,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -236,19 +230,10 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
@@ -543,7 +528,7 @@
   <dimension ref="C2:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,56 +552,56 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -630,23 +615,23 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11">
         <v>10</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15">
+      <c r="I5" s="11"/>
+      <c r="J5" s="12">
         <v>0</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="12" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D6">
-        <v>2045</v>
+        <v>2035</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -654,24 +639,24 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
-        <v>50</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11">
+        <v>10</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12">
         <v>0</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="12" t="s">
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -679,129 +664,154 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
-        <v>50</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11">
+        <v>10</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12">
         <v>0</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="12" t="s">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="D8">
+        <v>2045</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11">
+        <v>50</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="C9" s="5"/>
+      <c r="D9">
+        <v>2050</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11">
+        <v>50</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
     </row>
     <row r="17" spans="20:31" x14ac:dyDescent="0.3">
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>